<commit_message>
Updated Trello Dump and Sprint Log
</commit_message>
<xml_diff>
--- a/Documents/AFNT Trello Dump.xlsx
+++ b/Documents/AFNT Trello Dump.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AFA5C623-DA63-49A8-A704-D62C3D2E7A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:40009_{AFA5C623-DA63-49A8-A704-D62C3D2E7A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF215864-7C74-4B41-A9D8-E98DD5FD97B3}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390"/>
+    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4r2w1F7l - afnt-project" sheetId="1" r:id="rId1"/>
@@ -281,9 +281,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -870,46 +870,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -921,14 +894,32 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -939,14 +930,11 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -993,7 +981,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1008,26 +996,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8B8B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1368,11 +1336,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D74"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,27 +1352,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="3">
         <v>45403</v>
       </c>
       <c r="D2" s="2" t="b">
@@ -1412,11 +1380,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="3">
         <v>45403</v>
       </c>
       <c r="D3" s="2" t="b">
@@ -1424,11 +1392,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="3">
         <v>45403</v>
       </c>
       <c r="D4" s="2" t="b">
@@ -1436,11 +1404,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="3">
         <v>45403</v>
       </c>
       <c r="D5" s="2" t="b">
@@ -1448,13 +1416,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="21" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="3">
         <v>45352</v>
       </c>
       <c r="D6" s="2" t="b">
@@ -1462,11 +1430,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="3">
         <v>45366</v>
       </c>
       <c r="D7" s="2" t="b">
@@ -1474,11 +1442,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="3">
         <v>45402</v>
       </c>
       <c r="D8" s="2" t="b">
@@ -1486,11 +1454,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="3">
         <v>45403</v>
       </c>
       <c r="D9" s="2" t="b">
@@ -1498,25 +1466,25 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="3">
         <v>45406</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>80</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="3">
         <v>45394</v>
       </c>
       <c r="D11" s="2" t="b">
@@ -1524,11 +1492,11 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="3">
         <v>45395</v>
       </c>
       <c r="D12" s="2" t="b">
@@ -1536,11 +1504,11 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="3">
         <v>45402</v>
       </c>
       <c r="D13" s="2" t="b">
@@ -1548,13 +1516,13 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="3">
         <v>45323</v>
       </c>
       <c r="D14" s="2" t="b">
@@ -1562,11 +1530,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="3">
         <v>45323</v>
       </c>
       <c r="D15" s="2" t="b">
@@ -1574,11 +1542,11 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="3">
         <v>45323</v>
       </c>
       <c r="D16" s="2" t="b">
@@ -1586,11 +1554,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="3">
         <v>45327</v>
       </c>
       <c r="D17" s="2" t="b">
@@ -1598,11 +1566,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="3">
         <v>45327</v>
       </c>
       <c r="D18" s="2" t="b">
@@ -1610,11 +1578,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="3">
         <v>45341</v>
       </c>
       <c r="D19" s="2" t="b">
@@ -1622,11 +1590,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="3">
         <v>45342</v>
       </c>
       <c r="D20" s="2" t="b">
@@ -1634,11 +1602,11 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="3">
         <v>45343</v>
       </c>
       <c r="D21" s="2" t="b">
@@ -1646,11 +1614,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="3">
         <v>45351</v>
       </c>
       <c r="D22" s="2" t="b">
@@ -1658,11 +1626,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="3">
         <v>45353</v>
       </c>
       <c r="D23" s="2" t="b">
@@ -1670,11 +1638,11 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="3">
         <v>45353</v>
       </c>
       <c r="D24" s="2" t="b">
@@ -1682,11 +1650,11 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="3">
         <v>45358</v>
       </c>
       <c r="D25" s="2" t="b">
@@ -1694,11 +1662,11 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="3">
         <v>45359</v>
       </c>
       <c r="D26" s="2" t="b">
@@ -1706,11 +1674,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="3">
         <v>45373</v>
       </c>
       <c r="D27" s="2" t="b">
@@ -1718,13 +1686,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="3">
         <v>45294</v>
       </c>
       <c r="D28" s="2" t="b">
@@ -1732,11 +1700,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="3">
         <v>45301</v>
       </c>
       <c r="D29" s="2" t="b">
@@ -1744,11 +1712,11 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="3">
         <v>45301</v>
       </c>
       <c r="D30" s="2" t="b">
@@ -1756,11 +1724,11 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="3">
         <v>45307</v>
       </c>
       <c r="D31" s="2" t="b">
@@ -1768,11 +1736,11 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="3">
         <v>45309</v>
       </c>
       <c r="D32" s="2" t="b">
@@ -1780,11 +1748,11 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="3">
         <v>45312</v>
       </c>
       <c r="D33" s="2" t="b">
@@ -1792,11 +1760,11 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="3">
         <v>45312</v>
       </c>
       <c r="D34" s="2" t="b">
@@ -1804,11 +1772,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="3">
         <v>45313</v>
       </c>
       <c r="D35" s="2" t="b">
@@ -1816,11 +1784,11 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="3">
         <v>45313</v>
       </c>
       <c r="D36" s="2" t="b">
@@ -1828,11 +1796,11 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="3">
         <v>45315</v>
       </c>
       <c r="D37" s="2" t="b">
@@ -1840,11 +1808,11 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="3">
         <v>45315</v>
       </c>
       <c r="D38" s="2" t="b">
@@ -1852,13 +1820,13 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="18" t="s">
         <v>83</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="3">
         <v>45208</v>
       </c>
       <c r="D39" s="2" t="b">
@@ -1866,11 +1834,11 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="3">
         <v>45224</v>
       </c>
       <c r="D40" s="2" t="b">
@@ -1878,11 +1846,11 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C41" s="3">
         <v>45234</v>
       </c>
       <c r="D41" s="2" t="b">
@@ -1890,11 +1858,11 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="3">
         <v>45236</v>
       </c>
       <c r="D42" s="2" t="b">
@@ -1902,11 +1870,11 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="22"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C43" s="3">
         <v>45236</v>
       </c>
       <c r="D43" s="2" t="b">
@@ -1914,11 +1882,11 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="22"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C44" s="3">
         <v>45262</v>
       </c>
       <c r="D44" s="2" t="b">
@@ -1926,11 +1894,11 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="22"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="3">
         <v>45274</v>
       </c>
       <c r="D45" s="2" t="b">
@@ -1938,11 +1906,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="24">
+      <c r="C46" s="3">
         <v>45275</v>
       </c>
       <c r="D46" s="2" t="b">
@@ -1950,11 +1918,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="24">
+      <c r="C47" s="3">
         <v>45275</v>
       </c>
       <c r="D47" s="2" t="b">
@@ -1962,11 +1930,11 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="22"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="24">
+      <c r="C48" s="3">
         <v>45275</v>
       </c>
       <c r="D48" s="2" t="b">
@@ -1974,11 +1942,11 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="22"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="3">
         <v>45280</v>
       </c>
       <c r="D49" s="2" t="b">
@@ -1986,11 +1954,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="22"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="3">
         <v>45280</v>
       </c>
       <c r="D50" s="2" t="b">
@@ -1998,11 +1966,11 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="24">
+      <c r="C51" s="3">
         <v>45281</v>
       </c>
       <c r="D51" s="2" t="b">
@@ -2010,11 +1978,11 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C52" s="3">
         <v>45285</v>
       </c>
       <c r="D52" s="2" t="b">
@@ -2022,11 +1990,11 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="24">
+      <c r="C53" s="3">
         <v>45285</v>
       </c>
       <c r="D53" s="2" t="b">
@@ -2034,11 +2002,11 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="24">
+      <c r="C54" s="3">
         <v>45285</v>
       </c>
       <c r="D54" s="2" t="b">
@@ -2046,11 +2014,11 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="22"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C55" s="3">
         <v>45286</v>
       </c>
       <c r="D55" s="2" t="b">
@@ -2058,11 +2026,11 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="22"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="24">
+      <c r="C56" s="3">
         <v>45286</v>
       </c>
       <c r="D56" s="2" t="b">
@@ -2070,11 +2038,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="22"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C57" s="24">
+      <c r="C57" s="3">
         <v>45307</v>
       </c>
       <c r="D57" s="2" t="b">
@@ -2082,11 +2050,11 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="22"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C58" s="24">
+      <c r="C58" s="3">
         <v>45307</v>
       </c>
       <c r="D58" s="2" t="b">
@@ -2094,11 +2062,11 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="23"/>
+      <c r="A59" s="20"/>
       <c r="B59" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="24">
+      <c r="C59" s="3">
         <v>45306</v>
       </c>
       <c r="D59" s="2" t="b">
@@ -2106,13 +2074,13 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="24">
+      <c r="C60" s="3">
         <v>45208</v>
       </c>
       <c r="D60" s="2" t="b">
@@ -2120,11 +2088,11 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="16"/>
+      <c r="A61" s="7"/>
       <c r="B61" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="24">
+      <c r="C61" s="3">
         <v>45215</v>
       </c>
       <c r="D61" s="2" t="b">
@@ -2132,11 +2100,11 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="16"/>
+      <c r="A62" s="7"/>
       <c r="B62" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C62" s="24">
+      <c r="C62" s="3">
         <v>45215</v>
       </c>
       <c r="D62" s="2" t="b">
@@ -2144,11 +2112,11 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="16"/>
+      <c r="A63" s="7"/>
       <c r="B63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="24">
+      <c r="C63" s="3">
         <v>45218</v>
       </c>
       <c r="D63" s="2" t="b">
@@ -2156,11 +2124,11 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="16"/>
+      <c r="A64" s="7"/>
       <c r="B64" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="24">
+      <c r="C64" s="3">
         <v>45222</v>
       </c>
       <c r="D64" s="2" t="b">
@@ -2168,11 +2136,11 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="16"/>
+      <c r="A65" s="7"/>
       <c r="B65" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="24">
+      <c r="C65" s="3">
         <v>45229</v>
       </c>
       <c r="D65" s="2" t="b">
@@ -2180,11 +2148,11 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="16"/>
+      <c r="A66" s="7"/>
       <c r="B66" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C66" s="24">
+      <c r="C66" s="3">
         <v>45236</v>
       </c>
       <c r="D66" s="2" t="b">
@@ -2192,11 +2160,11 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="16"/>
+      <c r="A67" s="7"/>
       <c r="B67" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="24">
+      <c r="C67" s="3">
         <v>45281</v>
       </c>
       <c r="D67" s="2" t="b">
@@ -2204,11 +2172,11 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="16"/>
+      <c r="A68" s="7"/>
       <c r="B68" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="24">
+      <c r="C68" s="3">
         <v>44938</v>
       </c>
       <c r="D68" s="2" t="b">
@@ -2216,11 +2184,11 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="16"/>
+      <c r="A69" s="7"/>
       <c r="B69" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C69" s="24">
+      <c r="C69" s="3">
         <v>45316</v>
       </c>
       <c r="D69" s="2" t="b">
@@ -2228,11 +2196,11 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="16"/>
+      <c r="A70" s="7"/>
       <c r="B70" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C70" s="24">
+      <c r="C70" s="3">
         <v>45331</v>
       </c>
       <c r="D70" s="2" t="b">
@@ -2240,11 +2208,11 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="16"/>
+      <c r="A71" s="7"/>
       <c r="B71" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C71" s="24">
+      <c r="C71" s="3">
         <v>45345</v>
       </c>
       <c r="D71" s="2" t="b">
@@ -2252,11 +2220,11 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="16"/>
+      <c r="A72" s="7"/>
       <c r="B72" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C72" s="24">
+      <c r="C72" s="3">
         <v>45378</v>
       </c>
       <c r="D72" s="2" t="b">
@@ -2264,11 +2232,11 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="16"/>
+      <c r="A73" s="7"/>
       <c r="B73" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C73" s="24">
+      <c r="C73" s="3">
         <v>45401</v>
       </c>
       <c r="D73" s="2" t="b">
@@ -2276,11 +2244,11 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
+      <c r="A74" s="8"/>
       <c r="B74" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C74" s="24">
+      <c r="C74" s="3">
         <v>45405</v>
       </c>
       <c r="D74" s="2" t="b">
@@ -2291,11 +2259,11 @@
   <mergeCells count="7">
     <mergeCell ref="A60:A74"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A27"/>
     <mergeCell ref="A28:A38"/>
     <mergeCell ref="A39:A59"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">

</xml_diff>